<commit_message>
added some README-content (still a lot to do)
</commit_message>
<xml_diff>
--- a/Server/Classification/Results/Result_3DRNN_LSTM_FINAL_4a1c5b1f-2156-4712-aadf-6b61aabc1477.xlsx
+++ b/Server/Classification/Results/Result_3DRNN_LSTM_FINAL_4a1c5b1f-2156-4712-aadf-6b61aabc1477.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NUI_4.0\Server\Classification\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="3DRNN_LSTM_FINAL" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -142,8 +147,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,15 +190,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -235,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -267,9 +280,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -301,6 +332,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -476,17 +525,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AB31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AB40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="O30" sqref="O30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -494,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -502,7 +553,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -510,7 +561,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -518,7 +569,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -526,7 +577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -534,7 +585,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -542,7 +593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -550,15 +601,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>5e-05</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -566,7 +617,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -574,7 +625,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,7 +633,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -590,7 +641,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -598,7 +649,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -606,7 +657,7 @@
         <v>40603</v>
       </c>
     </row>
-    <row r="17" spans="1:28">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>21</v>
       </c>
@@ -614,7 +665,7 @@
         <v>6987</v>
       </c>
     </row>
-    <row r="18" spans="1:28">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
@@ -622,12 +673,12 @@
         <v>1247.73</v>
       </c>
     </row>
-    <row r="19" spans="1:28">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:28">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
@@ -707,7 +758,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:28">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>0</v>
       </c>
@@ -715,7 +766,7 @@
         <v>39</v>
       </c>
       <c r="C21">
-        <v>0.9945613281809074</v>
+        <v>0.99456132818090737</v>
       </c>
       <c r="D21">
         <v>6987</v>
@@ -742,16 +793,16 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>597.92</v>
+        <v>597.91999999999996</v>
       </c>
       <c r="M21">
         <v>0</v>
       </c>
       <c r="N21">
-        <v>7.307796477107331e-05</v>
+        <v>7.3077964771073312E-5</v>
       </c>
       <c r="O21">
-        <v>0.00120627261761158</v>
+        <v>1.2062726176115799E-3</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
@@ -790,7 +841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:28">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -798,7 +849,7 @@
         <v>39</v>
       </c>
       <c r="C22">
-        <v>0.9947044511235151</v>
+        <v>0.99470445112351513</v>
       </c>
       <c r="D22">
         <v>6987</v>
@@ -831,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="N22">
-        <v>8.631125092506409e-05</v>
+        <v>8.6311250925064087E-5</v>
       </c>
       <c r="O22">
         <v>0</v>
@@ -873,7 +924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:28">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>40</v>
       </c>
@@ -914,7 +965,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:28">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q24" s="1">
         <v>3</v>
       </c>
@@ -952,7 +1003,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:28">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q25" s="1">
         <v>4</v>
       </c>
@@ -990,7 +1041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:28">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q26" s="1">
         <v>5</v>
       </c>
@@ -1028,7 +1079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:28">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q27" s="1">
         <v>6</v>
       </c>
@@ -1066,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:28">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q28" s="1">
         <v>7</v>
       </c>
@@ -1104,7 +1155,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:28">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q29" s="1">
         <v>8</v>
       </c>
@@ -1142,7 +1193,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:28">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q30" s="1">
         <v>9</v>
       </c>
@@ -1180,7 +1231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:28">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="Q31" s="1">
         <v>10</v>
       </c>
@@ -1216,6 +1267,22 @@
       </c>
       <c r="AB31">
         <v>6121</v>
+      </c>
+    </row>
+    <row r="39" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T39">
+        <f>SUM(R21:AB30)</f>
+        <v>866</v>
+      </c>
+      <c r="W39">
+        <f>SUM(AB21:AB30)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="20:23" x14ac:dyDescent="0.25">
+      <c r="T40">
+        <f>SUM(R21,S22,T23,U24,V25,W26,X27,Y28,Z29,AA30)</f>
+        <v>829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>